<commit_message>
fix: change testcase format
</commit_message>
<xml_diff>
--- a/testcase.xlsx
+++ b/testcase.xlsx
@@ -7,14 +7,14 @@
     <workbookView windowHeight="15040"/>
   </bookViews>
   <sheets>
-    <sheet name="testcase1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29">
   <si>
     <t>Dataset</t>
   </si>
@@ -74,6 +74,24 @@
   </si>
   <si>
     <t>Runtime GA-ACO Percobaan 3</t>
+  </si>
+  <si>
+    <t>Image GA Percobaan 1</t>
+  </si>
+  <si>
+    <t>Image GA Percobaan 2</t>
+  </si>
+  <si>
+    <t>Image GA Percobaan 3</t>
+  </si>
+  <si>
+    <t>Image GA-ACO Percobaan 1</t>
+  </si>
+  <si>
+    <t>Image GA-ACO Percobaan 2</t>
+  </si>
+  <si>
+    <t>Image GA-ACO Percobaan 3</t>
   </si>
   <si>
     <t>t5.csv</t>
@@ -90,10 +108,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -119,11 +137,118 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -136,114 +261,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -271,181 +289,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -493,22 +511,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -524,15 +527,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -563,6 +557,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -576,142 +594,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1047,23 +1065,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:T10"/>
+  <dimension ref="A1:Z10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="Y6" sqref="Y6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="12.890625" customWidth="1"/>
-    <col min="2" max="2" width="12.5" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="10.0234375" customWidth="1"/>
-    <col min="8" max="8" width="10.8046875" customWidth="1"/>
-    <col min="9" max="20" width="14.3203125" customWidth="1"/>
+    <col min="1" max="1" width="14.3203125" customWidth="1"/>
+    <col min="8" max="8" width="11.453125" customWidth="1"/>
+    <col min="9" max="17" width="14.0625" customWidth="1"/>
+    <col min="18" max="20" width="17.9609375" customWidth="1"/>
+    <col min="21" max="26" width="14.0625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="29" customHeight="1" spans="1:20">
+    <row r="1" ht="48" customHeight="1" spans="1:26">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1123,11 +1140,29 @@
       </c>
       <c r="T1" s="1" t="s">
         <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B2">
         <v>10</v>
@@ -1153,7 +1188,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>50</v>
@@ -1179,7 +1214,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B4">
         <v>100</v>
@@ -1205,7 +1240,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B5">
         <v>10</v>
@@ -1231,7 +1266,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B6">
         <v>50</v>
@@ -1257,7 +1292,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B7">
         <v>100</v>
@@ -1283,7 +1318,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B8">
         <v>10</v>
@@ -1309,7 +1344,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B9">
         <v>50</v>
@@ -1335,7 +1370,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B10">
         <v>100</v>

</xml_diff>

<commit_message>
feature: add column testcase
</commit_message>
<xml_diff>
--- a/testcase.xlsx
+++ b/testcase.xlsx
@@ -14,18 +14,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30">
   <si>
     <t>Dataset</t>
   </si>
   <si>
-    <t>Generasi</t>
+    <t>Generasi GA</t>
+  </si>
+  <si>
+    <t>Populasi</t>
+  </si>
+  <si>
+    <t>Generasi ACO</t>
   </si>
   <si>
     <t>Jumlah Semut</t>
-  </si>
-  <si>
-    <t>Populasi</t>
   </si>
   <si>
     <t>Alpha</t>
@@ -108,10 +111,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -130,8 +133,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -145,39 +149,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -191,6 +172,60 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -200,45 +235,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -252,23 +256,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -283,13 +286,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -301,7 +406,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -313,157 +448,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -557,21 +560,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -589,150 +577,165 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1065,22 +1068,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:Z10"/>
+  <dimension ref="A1:AA10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="Y6" sqref="Y6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="14.3203125" customWidth="1"/>
-    <col min="8" max="8" width="11.453125" customWidth="1"/>
-    <col min="9" max="17" width="14.0625" customWidth="1"/>
-    <col min="18" max="20" width="17.9609375" customWidth="1"/>
-    <col min="21" max="26" width="14.0625" customWidth="1"/>
+    <col min="9" max="9" width="11.453125" customWidth="1"/>
+    <col min="10" max="18" width="14.0625" customWidth="1"/>
+    <col min="19" max="21" width="17.9609375" customWidth="1"/>
+    <col min="22" max="27" width="14.0625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="48" customHeight="1" spans="1:26">
+    <row r="1" ht="48" customHeight="1" spans="1:27">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1159,10 +1162,13 @@
       <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B2">
         <v>10</v>
@@ -1171,24 +1177,27 @@
         <v>5</v>
       </c>
       <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2">
         <v>5</v>
       </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
         <v>0.5</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B3">
         <v>50</v>
@@ -1197,24 +1206,27 @@
         <v>5</v>
       </c>
       <c r="D3">
+        <v>50</v>
+      </c>
+      <c r="E3">
         <v>5</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
         <v>0.5</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B4">
         <v>100</v>
@@ -1223,24 +1235,27 @@
         <v>5</v>
       </c>
       <c r="D4">
+        <v>100</v>
+      </c>
+      <c r="E4">
         <v>5</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
         <v>0.5</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B5">
         <v>10</v>
@@ -1252,21 +1267,24 @@
         <v>10</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
         <v>0.5</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B6">
         <v>50</v>
@@ -1275,24 +1293,27 @@
         <v>10</v>
       </c>
       <c r="D6">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
         <v>0.5</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B7">
         <v>100</v>
@@ -1301,96 +1322,108 @@
         <v>10</v>
       </c>
       <c r="D7">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
         <v>0.5</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B8">
         <v>10</v>
       </c>
       <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8">
         <v>100</v>
       </c>
-      <c r="D8">
-        <v>10</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
         <v>0.5</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B9">
         <v>50</v>
       </c>
       <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>50</v>
+      </c>
+      <c r="E9">
         <v>100</v>
       </c>
-      <c r="D9">
-        <v>10</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
         <v>0.5</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B10">
         <v>100</v>
       </c>
       <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10">
         <v>100</v>
       </c>
-      <c r="D10">
-        <v>10</v>
-      </c>
       <c r="E10">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
         <v>0.5</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add new chart 3 line
</commit_message>
<xml_diff>
--- a/testcase.xlsx
+++ b/testcase.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56">
   <si>
     <t>Dataset</t>
   </si>
@@ -167,6 +167,15 @@
   </si>
   <si>
     <t>Image GA-ACO 1 Line Percobaan 3</t>
+  </si>
+  <si>
+    <t>Image GA-ACO All Percobaan 1</t>
+  </si>
+  <si>
+    <t>Image GA-ACO All Percobaan 2</t>
+  </si>
+  <si>
+    <t>Image GA-ACO All Percobaan 3</t>
   </si>
   <si>
     <t>burma14.csv</t>
@@ -181,9 +190,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -202,16 +211,31 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -225,54 +249,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -301,6 +279,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -308,6 +287,59 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -317,30 +349,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -355,31 +364,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -391,37 +520,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -433,109 +544,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -564,13 +573,41 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -590,17 +627,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -610,15 +643,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -646,165 +670,150 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1137,10 +1146,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:AY6"/>
+  <dimension ref="A1:BB6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="AQ1" workbookViewId="0">
+      <selection activeCell="AY23" sqref="AY23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="5"/>
@@ -1155,9 +1164,12 @@
     <col min="49" max="49" width="15.4921875" customWidth="1"/>
     <col min="50" max="50" width="16.140625" customWidth="1"/>
     <col min="51" max="51" width="17.1796875" customWidth="1"/>
+    <col min="52" max="52" width="18.75" customWidth="1"/>
+    <col min="53" max="53" width="15.1015625" customWidth="1"/>
+    <col min="54" max="54" width="16.2734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="48" customHeight="1" spans="1:51">
+    <row r="1" ht="48" customHeight="1" spans="1:54">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1310,11 +1322,20 @@
       </c>
       <c r="AY1" s="1" t="s">
         <v>50</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B2">
         <v>10</v>
@@ -1343,7 +1364,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B3">
         <v>50</v>
@@ -1372,7 +1393,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B4">
         <v>100</v>
@@ -1401,7 +1422,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B5">
         <v>10</v>
@@ -1430,7 +1451,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B6">
         <v>50</v>

</xml_diff>

<commit_message>
add column number testcase v1 v2
</commit_message>
<xml_diff>
--- a/testcase.xlsx
+++ b/testcase.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57">
+  <si>
+    <t>No.</t>
+  </si>
   <si>
     <t>Dataset</t>
   </si>
@@ -190,9 +193,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -211,6 +214,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -226,9 +244,76 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -249,18 +334,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -271,89 +357,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -364,31 +367,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -400,37 +535,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -442,109 +547,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -573,6 +576,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -584,15 +605,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -612,17 +624,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -634,24 +640,6 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -670,150 +658,165 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1146,30 +1149,30 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:BB6"/>
+  <dimension ref="A1:BC6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AQ1" workbookViewId="0">
-      <selection activeCell="AY23" sqref="AY23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="5"/>
   <cols>
-    <col min="1" max="1" width="14.3203125" customWidth="1"/>
-    <col min="9" max="9" width="11.453125" customWidth="1"/>
-    <col min="10" max="32" width="14.0625" customWidth="1"/>
-    <col min="33" max="36" width="17.9609375" customWidth="1"/>
-    <col min="37" max="45" width="14.0625" customWidth="1"/>
-    <col min="46" max="47" width="16.796875" customWidth="1"/>
-    <col min="48" max="48" width="16.7890625" customWidth="1"/>
-    <col min="49" max="49" width="15.4921875" customWidth="1"/>
-    <col min="50" max="50" width="16.140625" customWidth="1"/>
-    <col min="51" max="51" width="17.1796875" customWidth="1"/>
-    <col min="52" max="52" width="18.75" customWidth="1"/>
-    <col min="53" max="53" width="15.1015625" customWidth="1"/>
-    <col min="54" max="54" width="16.2734375" customWidth="1"/>
+    <col min="2" max="2" width="14.3203125" customWidth="1"/>
+    <col min="10" max="10" width="11.453125" customWidth="1"/>
+    <col min="11" max="33" width="14.0625" customWidth="1"/>
+    <col min="34" max="37" width="17.9609375" customWidth="1"/>
+    <col min="38" max="46" width="14.0625" customWidth="1"/>
+    <col min="47" max="48" width="16.796875" customWidth="1"/>
+    <col min="49" max="49" width="16.7890625" customWidth="1"/>
+    <col min="50" max="50" width="15.4921875" customWidth="1"/>
+    <col min="51" max="51" width="16.140625" customWidth="1"/>
+    <col min="52" max="52" width="17.1796875" customWidth="1"/>
+    <col min="53" max="53" width="18.75" customWidth="1"/>
+    <col min="54" max="54" width="15.1015625" customWidth="1"/>
+    <col min="55" max="55" width="16.2734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="48" customHeight="1" spans="1:54">
+    <row r="1" ht="48" customHeight="1" spans="1:55">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1332,13 +1335,16 @@
       <c r="BB1" s="1" t="s">
         <v>53</v>
       </c>
+      <c r="BC1" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2">
-        <v>10</v>
+    <row r="2" spans="1:10">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -1350,82 +1356,91 @@
         <v>10</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
         <v>0.5</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3">
+    <row r="3" spans="1:10">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3">
         <v>50</v>
       </c>
-      <c r="C3">
-        <v>10</v>
-      </c>
       <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3">
         <v>50</v>
       </c>
-      <c r="E3">
-        <v>10</v>
-      </c>
       <c r="F3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
         <v>0.5</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4">
+    <row r="4" spans="1:10">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4">
         <v>100</v>
       </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
       <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
         <v>100</v>
       </c>
-      <c r="E4">
-        <v>10</v>
-      </c>
       <c r="F4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
       <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
         <v>0.5</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5">
-        <v>10</v>
+    <row r="5" spans="1:10">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
       </c>
       <c r="C5">
         <v>10</v>
@@ -1434,47 +1449,53 @@
         <v>10</v>
       </c>
       <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5">
         <v>100</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
       </c>
       <c r="G5">
         <v>1</v>
       </c>
       <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
         <v>0.5</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6">
+    <row r="6" spans="1:10">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6">
         <v>50</v>
       </c>
-      <c r="C6">
-        <v>10</v>
-      </c>
       <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
         <v>25</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>100</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
       </c>
       <c r="G6">
         <v>1</v>
       </c>
       <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
         <v>0.5</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>10</v>
       </c>
     </row>

</xml_diff>